<commit_message>
I think this should work much faster, legit.
</commit_message>
<xml_diff>
--- a/capture_test.xlsx
+++ b/capture_test.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -505,10 +508,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44952</v>
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>44966</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>44952</v>
@@ -538,16 +541,16 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>44952</v>
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>44966</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>44952</v>
+        <v>44966</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -571,16 +574,16 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>44952</v>
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>44966</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>44952</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -604,10 +607,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>44952</v>
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>44966</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>44952</v>

</xml_diff>